<commit_message>
added balance sheets MSTR
</commit_message>
<xml_diff>
--- a/MSTR.xlsx
+++ b/MSTR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00686E84-7993-41A2-A7A6-DB1B45FE2D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6612697E-AF7D-47DB-B75F-B671EC4B5FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
   <si>
     <t>Price</t>
   </si>
@@ -371,9 +371,6 @@
     <t>change mc to daily</t>
   </si>
   <si>
-    <t>balance sheet</t>
-  </si>
-  <si>
     <t>EBITDA + Digital Impairment</t>
   </si>
   <si>
@@ -468,7 +465,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -502,9 +499,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -20458,11 +20454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596D9E16-B52A-4557-A315-6FB674626433}">
   <dimension ref="A1:AA65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U23" sqref="U23"/>
+      <selection pane="bottomRight" activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21100,7 +21096,6 @@
       <c r="R10" s="4">
         <v>5319</v>
       </c>
-      <c r="T10" s="20"/>
       <c r="X10" s="4">
         <v>23977</v>
       </c>
@@ -21170,9 +21165,7 @@
       <c r="R11" s="4">
         <v>13617</v>
       </c>
-      <c r="T11" s="19" t="s">
-        <v>103</v>
-      </c>
+      <c r="T11" s="20"/>
       <c r="X11" s="4">
         <v>49952</v>
       </c>
@@ -21200,7 +21193,7 @@
         <v>23989</v>
       </c>
       <c r="E12" s="9">
-        <f t="shared" ref="E12:W12" si="7">SUM(E8:E11)</f>
+        <f t="shared" ref="E12:R12" si="7">SUM(E8:E11)</f>
         <v>21736</v>
       </c>
       <c r="F12" s="9">
@@ -22170,7 +22163,7 @@
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" ref="C25:H25" si="17">C20+C16</f>
@@ -22201,7 +22194,7 @@
         <v>6035</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" ref="J25:R25" si="18">J20+J16</f>
+        <f t="shared" ref="J25:Q25" si="18">J20+J16</f>
         <v>-1843</v>
       </c>
       <c r="K25" s="9">
@@ -22236,26 +22229,26 @@
         <f>R20+R16</f>
         <v>-21406</v>
       </c>
-      <c r="X25" s="21">
+      <c r="X25" s="19">
         <f>X20+X16</f>
         <v>50745</v>
       </c>
-      <c r="Y25" s="21">
+      <c r="Y25" s="19">
         <f>Y20+Y16</f>
         <v>19232</v>
       </c>
-      <c r="Z25" s="21">
+      <c r="Z25" s="19">
         <f>Z20+Z16</f>
         <v>-36179</v>
       </c>
-      <c r="AA25" s="21">
+      <c r="AA25" s="19">
         <f>AA20+AA16</f>
         <v>-8674</v>
       </c>
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G26" s="14">
         <f>G7/C7-1</f>
@@ -22315,13 +22308,13 @@
         <v>-2.2511463264690779E-2</v>
       </c>
       <c r="AA26" s="14">
-        <f t="shared" ref="Z26:AA26" si="20">AA7/Z7-1</f>
+        <f t="shared" ref="AA26" si="20">AA7/Z7-1</f>
         <v>-6.0148538648890915E-3</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" s="14">
         <f>C12/C7</f>
@@ -22403,7 +22396,7 @@
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="14">
         <f>SUM(G12:G15)/SUM(C12:C15)-1</f>
@@ -22473,15 +22466,15 @@
       </c>
       <c r="C31" s="9">
         <f t="shared" ref="C31:Q31" si="25">C32+C33+C57-C42-C43-C46-C47-C44-C45</f>
-        <v>0</v>
+        <v>289327</v>
       </c>
       <c r="D31" s="9">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f>D32+D33+D57-D42-D43-D46-D47-D44-D45</f>
+        <v>292175</v>
       </c>
       <c r="E31" s="9">
         <f t="shared" si="25"/>
-        <v>409504.5</v>
+        <v>219698.5</v>
       </c>
       <c r="F31" s="9">
         <f t="shared" si="25"/>
@@ -22489,7 +22482,7 @@
       </c>
       <c r="G31" s="9">
         <f t="shared" si="25"/>
-        <v>5351820.4972799998</v>
+        <v>3490024.4972799998</v>
       </c>
       <c r="H31" s="9">
         <f t="shared" si="25"/>
@@ -22497,7 +22490,7 @@
       </c>
       <c r="I31" s="9">
         <f t="shared" si="25"/>
-        <v>4964768.2915199995</v>
+        <v>2615948.2915199995</v>
       </c>
       <c r="J31" s="9">
         <f>J32+J33+J57-J42-J43-J46-J47-J44-J45</f>
@@ -22505,31 +22498,31 @@
       </c>
       <c r="K31" s="9">
         <f t="shared" si="25"/>
-        <v>5892701.3182200007</v>
-      </c>
-      <c r="L31" s="9">
+        <v>3324903.3182200007</v>
+      </c>
+      <c r="L31" s="18">
         <f t="shared" si="25"/>
-        <v>2450665.1989799999</v>
-      </c>
-      <c r="M31" s="9">
+        <v>-122756.80102000013</v>
+      </c>
+      <c r="M31" s="18">
         <f t="shared" si="25"/>
-        <v>2532466.2999999998</v>
-      </c>
-      <c r="N31" s="9">
+        <v>-38020.700000000186</v>
+      </c>
+      <c r="N31" s="18">
         <f t="shared" si="25"/>
         <v>-451382.60000000009</v>
       </c>
       <c r="O31" s="9">
         <f t="shared" si="25"/>
-        <v>3985581.6</v>
+        <v>1593728.6</v>
       </c>
       <c r="P31" s="9">
         <f t="shared" si="25"/>
-        <v>4625059.90283</v>
+        <v>2242208.90283</v>
       </c>
       <c r="Q31" s="9">
         <f t="shared" si="25"/>
-        <v>4277436.7251500003</v>
+        <v>1876551.7251500003</v>
       </c>
       <c r="R31" s="9">
         <f>R32+R33+R57-R42-R43-R46-R47-R44-R45</f>
@@ -22556,31 +22549,53 @@
       <c r="B32" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="8">
+        <v>429276</v>
+      </c>
+      <c r="D32" s="8">
+        <v>420899</v>
+      </c>
+      <c r="E32" s="8">
+        <v>52653</v>
+      </c>
       <c r="F32" s="8">
         <v>59675</v>
       </c>
-      <c r="G32" s="8"/>
+      <c r="G32" s="8">
+        <v>82544</v>
+      </c>
       <c r="H32" s="8">
         <v>56399</v>
       </c>
-      <c r="I32" s="8"/>
+      <c r="I32" s="8">
+        <v>56975</v>
+      </c>
       <c r="J32" s="8">
         <f>Y32</f>
         <v>63356</v>
       </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="K32" s="8">
+        <v>92677</v>
+      </c>
+      <c r="L32" s="8">
+        <v>69386</v>
+      </c>
+      <c r="M32" s="8">
+        <v>60390</v>
+      </c>
       <c r="N32" s="8">
         <f t="shared" ref="N32:N39" si="27">Z32</f>
         <v>43835</v>
       </c>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
+      <c r="O32" s="8">
+        <v>94311</v>
+      </c>
+      <c r="P32" s="8">
+        <v>65968</v>
+      </c>
+      <c r="Q32" s="8">
+        <v>45009</v>
+      </c>
       <c r="R32" s="8">
         <v>46817</v>
       </c>
@@ -22600,31 +22615,55 @@
       <c r="B33" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="C33" s="8">
+        <f>2742+109946</f>
+        <v>112688</v>
+      </c>
+      <c r="D33" s="8">
+        <f>1221+109972</f>
+        <v>111193</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1231</v>
+      </c>
       <c r="F33" s="8">
         <v>1084</v>
       </c>
-      <c r="G33" s="8"/>
+      <c r="G33" s="8">
+        <v>1194</v>
+      </c>
       <c r="H33" s="8">
         <v>1205</v>
       </c>
-      <c r="I33" s="8"/>
+      <c r="I33" s="8">
+        <v>1149</v>
+      </c>
       <c r="J33" s="8">
         <f t="shared" ref="J33:J51" si="28">Y33</f>
         <v>1078</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="K33" s="8">
+        <v>6265</v>
+      </c>
+      <c r="L33" s="8">
+        <v>6155</v>
+      </c>
+      <c r="M33" s="8">
+        <v>6578</v>
+      </c>
       <c r="N33" s="8">
         <f t="shared" si="27"/>
         <v>7033</v>
       </c>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
+      <c r="O33" s="8">
+        <v>2153</v>
+      </c>
+      <c r="P33" s="8">
+        <v>2085</v>
+      </c>
+      <c r="Q33" s="8">
+        <v>1865</v>
+      </c>
       <c r="R33" s="8">
         <v>1856</v>
       </c>
@@ -22644,31 +22683,53 @@
       <c r="B34" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="C34" s="8">
+        <v>124935</v>
+      </c>
+      <c r="D34" s="8">
+        <v>123794</v>
+      </c>
+      <c r="E34" s="8">
+        <v>148512</v>
+      </c>
       <c r="F34" s="8">
         <v>197461</v>
       </c>
-      <c r="G34" s="8"/>
+      <c r="G34" s="8">
+        <v>150626</v>
+      </c>
       <c r="H34" s="8">
         <v>131516</v>
       </c>
-      <c r="I34" s="8"/>
+      <c r="I34" s="8">
+        <v>123748</v>
+      </c>
       <c r="J34" s="8">
         <f t="shared" si="28"/>
         <v>189280</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="K34" s="8">
+        <v>126930</v>
+      </c>
+      <c r="L34" s="8">
+        <v>118645</v>
+      </c>
+      <c r="M34" s="8">
+        <v>109926</v>
+      </c>
       <c r="N34" s="8">
         <f t="shared" si="27"/>
         <v>189280</v>
       </c>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
+      <c r="O34" s="8">
+        <v>139178</v>
+      </c>
+      <c r="P34" s="8">
+        <v>121901</v>
+      </c>
+      <c r="Q34" s="8">
+        <v>128650</v>
+      </c>
       <c r="R34" s="8">
         <v>183815</v>
       </c>
@@ -22688,31 +22749,53 @@
       <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="C35" s="8">
+        <v>26163</v>
+      </c>
+      <c r="D35" s="8">
+        <v>16887</v>
+      </c>
+      <c r="E35" s="8">
+        <v>16040</v>
+      </c>
       <c r="F35" s="8">
         <v>14400</v>
       </c>
-      <c r="G35" s="8"/>
+      <c r="G35" s="8">
+        <v>16390</v>
+      </c>
       <c r="H35" s="8">
         <v>19338</v>
       </c>
-      <c r="I35" s="8"/>
+      <c r="I35" s="8">
+        <v>15750</v>
+      </c>
       <c r="J35" s="8">
         <f t="shared" si="28"/>
         <v>14251</v>
       </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
+      <c r="K35" s="8">
+        <v>21116</v>
+      </c>
+      <c r="L35" s="8">
+        <v>25496</v>
+      </c>
+      <c r="M35" s="8">
+        <v>25399</v>
+      </c>
       <c r="N35" s="8">
         <f t="shared" si="27"/>
         <v>24418</v>
       </c>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
+      <c r="O35" s="8">
+        <v>24034</v>
+      </c>
+      <c r="P35" s="8">
+        <v>19680</v>
+      </c>
+      <c r="Q35" s="8">
+        <v>24041</v>
+      </c>
       <c r="R35" s="8">
         <v>35407</v>
       </c>
@@ -22732,31 +22815,53 @@
       <c r="B36" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="C36" s="8">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
+        <v>380758</v>
+      </c>
       <c r="F36" s="8">
         <v>1054302</v>
       </c>
-      <c r="G36" s="8"/>
+      <c r="G36" s="8">
+        <v>1946582</v>
+      </c>
       <c r="H36" s="8">
         <v>2051039</v>
       </c>
-      <c r="I36" s="8"/>
+      <c r="I36" s="8">
+        <v>2405739</v>
+      </c>
       <c r="J36" s="8">
         <f t="shared" si="28"/>
         <v>2850210</v>
       </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="K36" s="8">
+        <v>2895619</v>
+      </c>
+      <c r="L36" s="8">
+        <v>1987781</v>
+      </c>
+      <c r="M36" s="8">
+        <v>1993032</v>
+      </c>
       <c r="N36" s="8">
         <f t="shared" si="27"/>
         <v>1840028</v>
       </c>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
+      <c r="O36" s="8">
+        <v>2000392</v>
+      </c>
+      <c r="P36" s="8">
+        <v>2323252</v>
+      </c>
+      <c r="Q36" s="8">
+        <v>2451374</v>
+      </c>
       <c r="R36" s="8">
         <v>3626476</v>
       </c>
@@ -22776,31 +22881,53 @@
       <c r="B37" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="C37" s="8">
+        <v>47623</v>
+      </c>
+      <c r="D37" s="8">
+        <v>45300</v>
+      </c>
+      <c r="E37" s="8">
+        <v>45473</v>
+      </c>
       <c r="F37" s="8">
         <v>42975</v>
       </c>
-      <c r="G37" s="8"/>
+      <c r="G37" s="8">
+        <v>41091</v>
+      </c>
       <c r="H37" s="8">
         <v>39659</v>
       </c>
-      <c r="I37" s="8"/>
+      <c r="I37" s="8">
+        <v>38133</v>
+      </c>
       <c r="J37" s="8">
         <f t="shared" si="28"/>
         <v>36587</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
+      <c r="K37" s="8">
+        <v>35680</v>
+      </c>
+      <c r="L37" s="8">
+        <v>34580</v>
+      </c>
+      <c r="M37" s="8">
+        <v>33033</v>
+      </c>
       <c r="N37" s="8">
         <f t="shared" si="27"/>
         <v>32311</v>
       </c>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
+      <c r="O37" s="8">
+        <v>31338</v>
+      </c>
+      <c r="P37" s="8">
+        <v>30507</v>
+      </c>
+      <c r="Q37" s="8">
+        <v>30192</v>
+      </c>
       <c r="R37" s="8">
         <v>28941</v>
       </c>
@@ -22820,31 +22947,53 @@
       <c r="B38" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="C38" s="8">
+        <v>82690</v>
+      </c>
+      <c r="D38" s="8">
+        <v>81543</v>
+      </c>
+      <c r="E38" s="8">
+        <v>79296</v>
+      </c>
       <c r="F38" s="8">
         <v>73597</v>
       </c>
-      <c r="G38" s="8"/>
+      <c r="G38" s="8">
+        <v>71357</v>
+      </c>
       <c r="H38" s="8">
         <v>70340</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="8">
+        <v>68755</v>
+      </c>
       <c r="J38" s="8">
         <f t="shared" si="28"/>
         <v>66760</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+      <c r="K38" s="8">
+        <v>64637</v>
+      </c>
+      <c r="L38" s="8">
+        <v>65169</v>
+      </c>
+      <c r="M38" s="8">
+        <v>62902</v>
+      </c>
       <c r="N38" s="8">
         <f t="shared" si="27"/>
         <v>61299</v>
       </c>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
+      <c r="O38" s="8">
+        <v>59655</v>
+      </c>
+      <c r="P38" s="8">
+        <v>58264</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>54542</v>
+      </c>
       <c r="R38" s="8">
         <v>57343</v>
       </c>
@@ -22864,31 +23013,53 @@
       <c r="B39" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="C39" s="8">
+        <v>7757</v>
+      </c>
+      <c r="D39" s="8">
+        <v>14596</v>
+      </c>
+      <c r="E39" s="8">
+        <v>15405</v>
+      </c>
       <c r="F39" s="8">
         <v>15615</v>
       </c>
-      <c r="G39" s="8"/>
+      <c r="G39" s="8">
+        <v>15013</v>
+      </c>
       <c r="H39" s="8">
         <v>15756</v>
       </c>
-      <c r="I39" s="8"/>
+      <c r="I39" s="8">
+        <v>14857</v>
+      </c>
       <c r="J39" s="8">
         <f t="shared" si="28"/>
         <v>15820</v>
       </c>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
+      <c r="K39" s="8">
+        <v>18181</v>
+      </c>
+      <c r="L39" s="8">
+        <v>17786</v>
+      </c>
+      <c r="M39" s="8">
+        <v>20992</v>
+      </c>
       <c r="N39" s="8">
         <f t="shared" si="27"/>
         <v>23916</v>
       </c>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
+      <c r="O39" s="8">
+        <v>23825</v>
+      </c>
+      <c r="P39" s="8">
+        <v>22421</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>24156</v>
+      </c>
       <c r="R39" s="8">
         <v>24300</v>
       </c>
@@ -22908,31 +23079,53 @@
       <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="C40" s="8">
+        <v>18139</v>
+      </c>
+      <c r="D40" s="8">
+        <v>18834</v>
+      </c>
+      <c r="E40" s="8">
+        <v>33537</v>
+      </c>
       <c r="F40" s="8">
         <v>6503</v>
       </c>
-      <c r="G40" s="8"/>
+      <c r="G40" s="8">
+        <v>118272</v>
+      </c>
       <c r="H40" s="8">
         <v>239107</v>
       </c>
-      <c r="I40" s="8"/>
+      <c r="I40" s="8">
+        <v>261138</v>
+      </c>
       <c r="J40" s="8">
         <f t="shared" si="28"/>
         <v>319782</v>
       </c>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+      <c r="K40" s="8">
+        <v>377282</v>
+      </c>
+      <c r="L40" s="8">
+        <v>243367</v>
+      </c>
+      <c r="M40" s="8">
+        <v>233034</v>
+      </c>
       <c r="N40" s="8">
         <f>Z40</f>
         <v>188152</v>
       </c>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
+      <c r="O40" s="8">
+        <v>651516</v>
+      </c>
+      <c r="P40" s="8">
+        <v>719026</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>614112</v>
+      </c>
       <c r="R40" s="8">
         <v>757573</v>
       </c>
@@ -22952,14 +23145,17 @@
       <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C41" s="11"/>
+      <c r="C41" s="11">
+        <f>SUM(C32:C40)</f>
+        <v>849271</v>
+      </c>
       <c r="D41" s="11">
         <f>SUM(D32:D40)</f>
-        <v>0</v>
+        <v>833046</v>
       </c>
       <c r="E41" s="11">
         <f t="shared" ref="E41:R41" si="30">SUM(E32:E40)</f>
-        <v>0</v>
+        <v>772905</v>
       </c>
       <c r="F41" s="11">
         <f t="shared" si="30"/>
@@ -22967,15 +23163,15 @@
       </c>
       <c r="G41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>2443069</v>
       </c>
       <c r="H41" s="11">
         <f t="shared" si="30"/>
         <v>2624359</v>
       </c>
       <c r="I41" s="11">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f>SUM(I32:I40)</f>
+        <v>2986244</v>
       </c>
       <c r="J41" s="11">
         <f>SUM(J32:J40)</f>
@@ -22983,15 +23179,15 @@
       </c>
       <c r="K41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>3638387</v>
       </c>
       <c r="L41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>2568365</v>
       </c>
       <c r="M41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>2545286</v>
       </c>
       <c r="N41" s="11">
         <f t="shared" si="30"/>
@@ -22999,15 +23195,15 @@
       </c>
       <c r="O41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>3026402</v>
       </c>
       <c r="P41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>3363104</v>
       </c>
       <c r="Q41" s="11">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>3373941</v>
       </c>
       <c r="R41" s="11">
         <f t="shared" si="30"/>
@@ -23034,31 +23230,53 @@
       <c r="B42" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="C42" s="8">
+        <v>32539</v>
+      </c>
+      <c r="D42" s="8">
+        <v>31468</v>
+      </c>
+      <c r="E42" s="8">
+        <v>38668</v>
+      </c>
       <c r="F42" s="8">
         <v>45119</v>
       </c>
-      <c r="G42" s="8"/>
+      <c r="G42" s="8">
+        <v>39816</v>
+      </c>
       <c r="H42" s="8">
         <v>41236</v>
       </c>
-      <c r="I42" s="8"/>
+      <c r="I42" s="8">
+        <v>45454</v>
+      </c>
       <c r="J42" s="8">
         <f>Y42</f>
         <v>46084</v>
       </c>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
+      <c r="K42" s="8">
+        <v>44388</v>
+      </c>
+      <c r="L42" s="8">
+        <v>35960</v>
+      </c>
+      <c r="M42" s="8">
+        <v>36846</v>
+      </c>
       <c r="N42" s="8">
         <f>Z42</f>
         <v>42976</v>
       </c>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
+      <c r="O42" s="8">
+        <v>50604</v>
+      </c>
+      <c r="P42" s="8">
+        <v>33660</v>
+      </c>
+      <c r="Q42" s="8">
+        <v>34306</v>
+      </c>
       <c r="R42" s="8">
         <v>43090</v>
       </c>
@@ -23078,31 +23296,53 @@
       <c r="B43" t="s">
         <v>74</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="C43" s="8">
+        <v>35207</v>
+      </c>
+      <c r="D43" s="8">
+        <v>40806</v>
+      </c>
+      <c r="E43" s="8">
+        <v>44177</v>
+      </c>
       <c r="F43" s="8">
         <v>49249</v>
       </c>
-      <c r="G43" s="8"/>
+      <c r="G43" s="8">
+        <v>44824</v>
+      </c>
       <c r="H43" s="8">
         <v>50944</v>
       </c>
-      <c r="I43" s="8"/>
+      <c r="I43" s="8">
+        <v>47759</v>
+      </c>
       <c r="J43" s="8">
         <f t="shared" si="28"/>
         <v>54548</v>
       </c>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
+      <c r="K43" s="8">
+        <v>43726</v>
+      </c>
+      <c r="L43" s="8">
+        <v>47773</v>
+      </c>
+      <c r="M43" s="8">
+        <v>46346</v>
+      </c>
       <c r="N43" s="8">
         <f t="shared" ref="N43:N51" si="32">Z43</f>
         <v>53716</v>
       </c>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
+      <c r="O43" s="8">
+        <v>39199</v>
+      </c>
+      <c r="P43" s="8">
+        <v>41492</v>
+      </c>
+      <c r="Q43" s="8">
+        <v>43405</v>
+      </c>
       <c r="R43" s="8">
         <v>50045</v>
       </c>
@@ -23133,16 +23373,28 @@
         <f t="shared" si="28"/>
         <v>1493</v>
       </c>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
+      <c r="K44" s="8">
+        <v>10544</v>
+      </c>
+      <c r="L44" s="8">
+        <v>2269</v>
+      </c>
+      <c r="M44" s="8">
+        <v>11394</v>
+      </c>
       <c r="N44" s="8">
         <f t="shared" si="32"/>
         <v>2829</v>
       </c>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
+      <c r="O44" s="8">
+        <v>10368</v>
+      </c>
+      <c r="P44" s="8">
+        <v>1493</v>
+      </c>
+      <c r="Q44" s="8">
+        <v>10368</v>
+      </c>
       <c r="R44" s="8">
         <v>1493</v>
       </c>
@@ -23169,20 +23421,25 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="8">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
+      <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
+      <c r="M45" s="8">
+        <v>0</v>
+      </c>
       <c r="N45" s="8">
         <f t="shared" si="32"/>
         <v>454</v>
       </c>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
+      <c r="O45" s="8">
+        <v>460</v>
+      </c>
+      <c r="P45" s="8">
+        <v>468</v>
+      </c>
+      <c r="Q45" s="8">
+        <v>475</v>
+      </c>
       <c r="R45" s="8">
         <v>483</v>
       </c>
@@ -23202,31 +23459,53 @@
       <c r="B46" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="C46" s="8">
+        <v>184891</v>
+      </c>
+      <c r="D46" s="8">
+        <v>167643</v>
+      </c>
+      <c r="E46" s="8">
+        <v>160845</v>
+      </c>
       <c r="F46" s="8">
         <v>191250</v>
       </c>
-      <c r="G46" s="8"/>
+      <c r="G46" s="8">
+        <v>198980</v>
+      </c>
       <c r="H46" s="8">
         <v>182818</v>
       </c>
-      <c r="I46" s="8"/>
+      <c r="I46" s="8">
+        <v>160697</v>
+      </c>
       <c r="J46" s="8">
         <f t="shared" si="28"/>
         <v>209860</v>
       </c>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
+      <c r="K46" s="8">
+        <v>206217</v>
+      </c>
+      <c r="L46" s="8">
+        <v>188098</v>
+      </c>
+      <c r="M46" s="8">
+        <v>165934</v>
+      </c>
       <c r="N46" s="8">
         <f t="shared" si="32"/>
         <v>217428</v>
       </c>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
+      <c r="O46" s="8">
+        <v>211768</v>
+      </c>
+      <c r="P46" s="8">
+        <v>195817</v>
+      </c>
+      <c r="Q46" s="8">
+        <v>179167</v>
+      </c>
       <c r="R46" s="8">
         <v>228162</v>
       </c>
@@ -23252,25 +23531,41 @@
       <c r="F47" s="8">
         <v>486366</v>
       </c>
-      <c r="G47" s="8"/>
+      <c r="G47" s="8">
+        <v>1661914</v>
+      </c>
       <c r="H47" s="8">
         <v>2150927</v>
       </c>
-      <c r="I47" s="8"/>
+      <c r="I47" s="8">
+        <v>2153034</v>
+      </c>
       <c r="J47" s="8">
         <f t="shared" si="28"/>
         <v>2155151</v>
       </c>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
+      <c r="K47" s="8">
+        <v>2361865</v>
+      </c>
+      <c r="L47" s="8">
+        <v>2374863</v>
+      </c>
+      <c r="M47" s="8">
+        <v>2376935</v>
+      </c>
       <c r="N47" s="8">
         <f t="shared" si="32"/>
         <v>2378560</v>
       </c>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
+      <c r="O47" s="8">
+        <v>2175918</v>
+      </c>
+      <c r="P47" s="8">
+        <v>2177974</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>2180038</v>
+      </c>
       <c r="R47" s="8">
         <v>2182108</v>
       </c>
@@ -23290,31 +23585,53 @@
       <c r="B48" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="C48" s="8">
+        <v>3660</v>
+      </c>
+      <c r="D48" s="8">
+        <v>5910</v>
+      </c>
+      <c r="E48" s="8">
+        <v>11657</v>
+      </c>
       <c r="F48" s="8">
         <v>14662</v>
       </c>
-      <c r="G48" s="8"/>
+      <c r="G48" s="8">
+        <v>14517</v>
+      </c>
       <c r="H48" s="8">
         <v>7262</v>
       </c>
-      <c r="I48" s="8"/>
+      <c r="I48" s="8">
+        <v>8302</v>
+      </c>
       <c r="J48" s="8">
         <f t="shared" si="28"/>
         <v>8089</v>
       </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
+      <c r="K48" s="8">
+        <v>8236</v>
+      </c>
+      <c r="L48" s="8">
+        <v>8497</v>
+      </c>
+      <c r="M48" s="8">
+        <v>8754</v>
+      </c>
       <c r="N48" s="8">
         <f t="shared" si="32"/>
         <v>12763</v>
       </c>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
+      <c r="O48" s="8">
+        <v>11646</v>
+      </c>
+      <c r="P48" s="8">
+        <v>11244</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>7638</v>
+      </c>
       <c r="R48" s="8">
         <v>8524</v>
       </c>
@@ -23334,31 +23651,53 @@
       <c r="B49" t="s">
         <v>21</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="C49" s="8">
+        <v>100251</v>
+      </c>
+      <c r="D49" s="8">
+        <v>98283</v>
+      </c>
+      <c r="E49" s="8">
+        <v>95591</v>
+      </c>
       <c r="F49" s="8">
         <v>84328</v>
       </c>
-      <c r="G49" s="8"/>
+      <c r="G49" s="8">
+        <v>81849</v>
+      </c>
       <c r="H49" s="8">
         <v>80900</v>
       </c>
-      <c r="I49" s="8"/>
+      <c r="I49" s="8">
+        <v>78939</v>
+      </c>
       <c r="J49" s="8">
         <f t="shared" si="28"/>
         <v>76608</v>
       </c>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
+      <c r="K49" s="8">
+        <v>73956</v>
+      </c>
+      <c r="L49" s="8">
+        <v>72162</v>
+      </c>
+      <c r="M49" s="8">
+        <v>69278</v>
+      </c>
       <c r="N49" s="8">
         <f t="shared" si="32"/>
         <v>67344</v>
       </c>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
+      <c r="O49" s="8">
+        <v>65355</v>
+      </c>
+      <c r="P49" s="8">
+        <v>63814</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>59720</v>
+      </c>
       <c r="R49" s="8">
         <v>61086</v>
       </c>
@@ -23378,31 +23717,53 @@
       <c r="B50" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="C50" s="8">
+        <v>31273</v>
+      </c>
+      <c r="D50" s="8">
+        <v>30452</v>
+      </c>
+      <c r="E50" s="8">
+        <v>32651</v>
+      </c>
       <c r="F50" s="8">
         <v>33382</v>
       </c>
-      <c r="G50" s="8"/>
+      <c r="G50" s="8">
+        <v>34329</v>
+      </c>
       <c r="H50" s="8">
         <v>31040</v>
       </c>
-      <c r="I50" s="8"/>
+      <c r="I50" s="8">
+        <v>28934</v>
+      </c>
       <c r="J50" s="8">
         <f t="shared" si="28"/>
         <v>26224</v>
       </c>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
+      <c r="K50" s="8">
+        <v>26347</v>
+      </c>
+      <c r="L50" s="8">
+        <v>25706</v>
+      </c>
+      <c r="M50" s="8">
+        <v>30088</v>
+      </c>
       <c r="N50" s="8">
         <f t="shared" si="32"/>
         <v>17124</v>
       </c>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
+      <c r="O50" s="8">
+        <v>17675</v>
+      </c>
+      <c r="P50" s="8">
+        <v>17826</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>18231</v>
+      </c>
       <c r="R50" s="8">
         <v>22208</v>
       </c>
@@ -23422,31 +23783,53 @@
       <c r="B51" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="C51" s="8">
+        <v>24</v>
+      </c>
+      <c r="D51" s="8">
+        <v>24</v>
+      </c>
+      <c r="E51" s="8">
+        <v>24</v>
+      </c>
       <c r="F51" s="8">
         <v>8211</v>
       </c>
-      <c r="G51" s="8"/>
+      <c r="G51" s="8">
+        <v>1812</v>
+      </c>
       <c r="H51" s="8">
         <v>1813</v>
       </c>
-      <c r="I51" s="8"/>
+      <c r="I51" s="8">
+        <v>1811</v>
+      </c>
       <c r="J51" s="8">
         <f t="shared" si="28"/>
         <v>109</v>
       </c>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
+      <c r="K51" s="8">
+        <v>109</v>
+      </c>
+      <c r="L51" s="8">
+        <v>105</v>
+      </c>
+      <c r="M51" s="8">
+        <v>0</v>
+      </c>
       <c r="N51" s="8">
         <f t="shared" si="32"/>
         <v>198</v>
       </c>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
+      <c r="O51" s="8">
+        <v>198</v>
+      </c>
+      <c r="P51" s="8">
+        <v>198</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>198</v>
+      </c>
       <c r="R51" s="8">
         <v>357</v>
       </c>
@@ -23466,14 +23849,17 @@
       <c r="B52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="11"/>
+      <c r="C52" s="11">
+        <f>SUM(C42:C51)</f>
+        <v>387845</v>
+      </c>
       <c r="D52" s="11">
         <f>SUM(D42:D51)</f>
-        <v>0</v>
+        <v>374586</v>
       </c>
       <c r="E52" s="11">
         <f t="shared" ref="E52:R52" si="34">SUM(E42:E51)</f>
-        <v>0</v>
+        <v>383613</v>
       </c>
       <c r="F52" s="11">
         <f t="shared" si="34"/>
@@ -23481,7 +23867,7 @@
       </c>
       <c r="G52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2078041</v>
       </c>
       <c r="H52" s="11">
         <f t="shared" si="34"/>
@@ -23489,7 +23875,7 @@
       </c>
       <c r="I52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2524930</v>
       </c>
       <c r="J52" s="11">
         <f t="shared" si="34"/>
@@ -23497,15 +23883,15 @@
       </c>
       <c r="K52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2775388</v>
       </c>
       <c r="L52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2755433</v>
       </c>
       <c r="M52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2745575</v>
       </c>
       <c r="N52" s="11">
         <f t="shared" si="34"/>
@@ -23513,15 +23899,15 @@
       </c>
       <c r="O52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2583191</v>
       </c>
       <c r="P52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2543986</v>
       </c>
       <c r="Q52" s="11">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>2533546</v>
       </c>
       <c r="R52" s="11">
         <f t="shared" si="34"/>
@@ -23754,7 +24140,7 @@
         <v>917223.33104999992</v>
       </c>
       <c r="G58" s="12">
-        <f t="shared" ref="F58:R58" si="37">G57-G60</f>
+        <f t="shared" ref="G58:R58" si="37">G57-G60</f>
         <v>3140445.4972799998</v>
       </c>
       <c r="H58" s="12">
@@ -23915,7 +24301,7 @@
         <v>3160471</v>
       </c>
       <c r="J60" s="8">
-        <f t="shared" ref="J60:R60" si="39">I60+J64</f>
+        <f t="shared" ref="J60:Q60" si="39">I60+J64</f>
         <v>3751529</v>
       </c>
       <c r="K60" s="8">
@@ -24133,6 +24519,9 @@
     <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{FFD6FC28-FD87-4776-93D1-3783D6C7039D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N41 J41" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -24140,7 +24529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85EA0FE-1A7B-4E67-A576-244712A3E077}">
   <dimension ref="A1:K191"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>

</xml_diff>